<commit_message>
Correctly parses different tokens
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2109FA80-3D5C-694A-9B13-1BB57D2D7CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A86BA74-E997-264F-AAC9-324501B14E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
+    <workbookView xWindow="1640" yWindow="2320" windowWidth="28040" windowHeight="17440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>p</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Hello World</t>
   </si>
@@ -47,13 +44,22 @@
     <t>paragraph</t>
   </si>
   <si>
-    <t>// Ignore</t>
-  </si>
-  <si>
     <t>purple</t>
   </si>
   <si>
     <t>Hello Again</t>
+  </si>
+  <si>
+    <t>Let's try this out</t>
+  </si>
+  <si>
+    <t>hehe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     // Ignore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     p</t>
   </si>
 </sst>
 </file>
@@ -425,43 +431,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABFE800-D097-7545-8A42-4067DC28C4D0}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can now read command tokens
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A86BA74-E997-264F-AAC9-324501B14E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B720D6-CFC9-1C48-8CAA-701BBC3D22BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1640" yWindow="2320" windowWidth="28040" windowHeight="17440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Hello World</t>
   </si>
   <si>
-    <t>paragraph</t>
-  </si>
-  <si>
     <t>purple</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t xml:space="preserve">     p</t>
+  </si>
+  <si>
+    <t>PARAgrAPH</t>
   </si>
 </sst>
 </file>
@@ -434,14 +434,14 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -451,33 +451,33 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new style command. Can now process arguments
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75971DEA-C6D2-114B-B25A-42FFB182E424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61041773-8B3B-044C-8A06-462C9B2B5EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16960" windowHeight="20440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,36 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>paragraph</t>
+    <t>style</t>
   </si>
   <si>
-    <t>paRAgrAPH</t>
+    <t>font=Aptos</t>
   </si>
   <si>
-    <t xml:space="preserve">    p</t>
+    <t>Name=Text</t>
   </si>
   <si>
-    <t>smack my ass</t>
+    <t>PARENT  =null</t>
   </si>
   <si>
-    <t>like a drum!</t>
+    <t>coloR=   000000</t>
   </si>
   <si>
-    <t>papiiii</t>
-  </si>
-  <si>
-    <t>glug glug glug</t>
-  </si>
-  <si>
-    <t>// don't look at this shit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    yes daddy!!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    // aaughhgh!!!</t>
+    <t>siZE = 12</t>
   </si>
 </sst>
 </file>
@@ -450,120 +438,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABFE800-D097-7545-8A42-4067DC28C4D0}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>

</xml_diff>

<commit_message>
Can now add styles to Word doc
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61041773-8B3B-044C-8A06-462C9B2B5EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB31B98-22FB-A64D-9B72-03F745232376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="16960" windowHeight="20440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
@@ -50,10 +50,10 @@
     <t>PARENT  =null</t>
   </si>
   <si>
-    <t>coloR=   000000</t>
+    <t>siZE = 12</t>
   </si>
   <si>
-    <t>siZE = 12</t>
+    <t>coloR=   00ff00</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Can now apply styles to paragraphs
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB31B98-22FB-A64D-9B72-03F745232376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01052CB3-D2AC-7C47-B1D3-E95A4260DB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="16960" windowHeight="20440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>paragraph</t>
+  </si>
   <si>
     <t>style</t>
   </si>
@@ -44,16 +47,28 @@
     <t>font=Aptos</t>
   </si>
   <si>
-    <t>Name=Text</t>
-  </si>
-  <si>
     <t>PARENT  =null</t>
   </si>
   <si>
     <t>siZE = 12</t>
   </si>
   <si>
-    <t>coloR=   00ff00</t>
+    <t>This is a paragraph.</t>
+  </si>
+  <si>
+    <t>This is another paragraph.</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
+    <t>Name=Example</t>
+  </si>
+  <si>
+    <t>coloR=   0000ff</t>
+  </si>
+  <si>
+    <t>style=Example</t>
   </si>
 </sst>
 </file>
@@ -441,55 +456,65 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>

</xml_diff>

<commit_message>
Style names are now validated
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01052CB3-D2AC-7C47-B1D3-E95A4260DB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5052EFDA-1C8C-2245-8B9D-C01F00CB10A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="16960" windowHeight="20440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
@@ -62,13 +62,13 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
   </si>
   <si>
-    <t>Name=Example</t>
-  </si>
-  <si>
     <t>coloR=   0000ff</t>
   </si>
   <si>
-    <t>style=Example</t>
+    <t>Name=Smack My Ass</t>
+  </si>
+  <si>
+    <t>style=smack my ass</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,13 +466,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Now preserves empty paragraphs
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristian/Dropbox/Home/coding/xmlyze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C5951C-B362-244E-B4D6-B4AB5C91CA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42A7B78-7693-9E47-A1AD-610931889B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="16960" windowHeight="20440" xr2:uid="{21459283-2947-7E47-9D1F-CEB35E8C06FF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>paragraph</t>
   </si>
@@ -453,7 +453,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,31 +506,37 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>

</xml_diff>